<commit_message>
Asserted page header on new contacts page
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRM.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRM.xlsx
@@ -4,8 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Plan" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="NewContactDetails" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="NewDealsDetails" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="NewTaskDetails" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="NewContactDetails" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="NewDealsDetails" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="117">
   <si>
     <t>Create new contacts from excel file</t>
   </si>
@@ -33,6 +34,84 @@
     <t>format xpath with name taken from excel file</t>
   </si>
   <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Contacts</t>
+  </si>
+  <si>
+    <t>Deals</t>
+  </si>
+  <si>
+    <t>DueDate</t>
+  </si>
+  <si>
+    <t>CloseDate</t>
+  </si>
+  <si>
+    <t>Weekly</t>
+  </si>
+  <si>
+    <t>Sheetal</t>
+  </si>
+  <si>
+    <t>Pen Deal</t>
+  </si>
+  <si>
+    <t>07/08/2020 17:00</t>
+  </si>
+  <si>
+    <t>30/09/2020 17:00</t>
+  </si>
+  <si>
+    <t>Bi-weekly</t>
+  </si>
+  <si>
+    <t>Payal</t>
+  </si>
+  <si>
+    <t>Pencil Deal</t>
+  </si>
+  <si>
+    <t>14/08/2020 17:30</t>
+  </si>
+  <si>
+    <t>Fortnightly</t>
+  </si>
+  <si>
+    <t>Koyal</t>
+  </si>
+  <si>
+    <t>Sharpner Deal</t>
+  </si>
+  <si>
+    <t>15/08/2020 18:00</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Monal</t>
+  </si>
+  <si>
+    <t>Eraser Deal</t>
+  </si>
+  <si>
+    <t>31/08/2020 12:00</t>
+  </si>
+  <si>
+    <t>Quarterly</t>
+  </si>
+  <si>
+    <t>Rupal</t>
+  </si>
+  <si>
+    <t>Ruler Deal</t>
+  </si>
+  <si>
+    <t>31/12/2020 16:00</t>
+  </si>
+  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -213,12 +292,6 @@
     <t>2007</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Contacts</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -228,9 +301,6 @@
     <t>Christmas deal</t>
   </si>
   <si>
-    <t>Payal</t>
-  </si>
-  <si>
     <t>1250</t>
   </si>
   <si>
@@ -240,9 +310,6 @@
     <t>New Year deal</t>
   </si>
   <si>
-    <t>Sheetal</t>
-  </si>
-  <si>
     <t>1750</t>
   </si>
   <si>
@@ -252,9 +319,6 @@
     <t>Thanksgiving deal</t>
   </si>
   <si>
-    <t>Rupal</t>
-  </si>
-  <si>
     <t>1658</t>
   </si>
   <si>
@@ -288,9 +352,6 @@
     <t>Independence Day deal</t>
   </si>
   <si>
-    <t>Koyal</t>
-  </si>
-  <si>
     <t>36585</t>
   </si>
   <si>
@@ -298,9 +359,6 @@
   </si>
   <si>
     <t>Presidents Day Deal</t>
-  </si>
-  <si>
-    <t>Monal</t>
   </si>
   <si>
     <t>32145</t>
@@ -345,14 +403,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -360,9 +418,6 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -382,6 +437,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -617,7 +676,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -636,39 +695,159 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="4" max="4" width="15.57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
     <col customWidth="1" min="6" max="6" width="15.29"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -690,227 +869,227 @@
       <c r="AB1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>17</v>
+      <c r="A2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>27</v>
+      <c r="A3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>36</v>
+      <c r="A4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="H7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="D8" s="1" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -918,7 +1097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -933,138 +1112,138 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="C5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>93</v>
+        <v>21</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>62</v>
+        <v>114</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>97</v>
+        <v>25</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>